<commit_message>
feat: add series table
</commit_message>
<xml_diff>
--- a/docs/sodo_qh.xlsx
+++ b/docs/sodo_qh.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truon\Desktop\f5mobile-nuxtjs\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1356EC3-751B-4B20-A3E9-E83FC2657972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A55EFAA-8DE3-490D-AF93-2C52550D74DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{11496C9D-87F9-4847-A4DD-6E9F85763FD5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
   <si>
     <t>description</t>
   </si>
@@ -109,6 +109,33 @@
   </si>
   <si>
     <t>status</t>
+  </si>
+  <si>
+    <t>status_id</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>value</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>category_id</t>
+  </si>
+  <si>
+    <t>category</t>
+  </si>
+  <si>
+    <t>Series</t>
+  </si>
+  <si>
+    <t>series_id</t>
+  </si>
+  <si>
+    <t>series</t>
   </si>
 </sst>
 </file>
@@ -492,40 +519,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730279FF-5D8F-42BA-819F-46A5B9217A82}">
-  <dimension ref="A2:N12"/>
+  <dimension ref="A2:P19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.85546875" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
-    <col min="3" max="3" width="12.5703125" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" customWidth="1"/>
-    <col min="11" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" customWidth="1"/>
-    <col min="13" max="13" width="11.28515625" customWidth="1"/>
-    <col min="14" max="14" width="12.28515625" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.140625" customWidth="1"/>
+    <col min="10" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.28515625" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" customWidth="1"/>
+    <col min="16" max="16" width="12.28515625" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -556,76 +583,133 @@
       <c r="J3" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="K3" s="1" t="s">
+        <v>28</v>
+      </c>
       <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E7" s="2" t="s">
+      <c r="P3" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O5" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N6" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="P6" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="M7" s="2" t="s">
+      <c r="O8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E11" s="2" t="s">
+      <c r="P9" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O11" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N12" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="O12" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M11" s="2" t="s">
+      <c r="O14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L12" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="N12" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="O18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="14:16" x14ac:dyDescent="0.25">
+      <c r="N19" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="O19" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="P19" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: add endpoint product
</commit_message>
<xml_diff>
--- a/docs/sodo_qh.xlsx
+++ b/docs/sodo_qh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truon\Desktop\f5mobile-nuxtjs\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A55EFAA-8DE3-490D-AF93-2C52550D74DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2988F2BD-F939-491B-92D4-7AF93F1292EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{11496C9D-87F9-4847-A4DD-6E9F85763FD5}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="38">
   <si>
     <t>description</t>
   </si>
@@ -136,6 +136,9 @@
   </si>
   <si>
     <t>series</t>
+  </si>
+  <si>
+    <t>link</t>
   </si>
 </sst>
 </file>
@@ -201,10 +204,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -519,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730279FF-5D8F-42BA-819F-46A5B9217A82}">
-  <dimension ref="A2:P19"/>
+  <dimension ref="A2:Q19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,29 +534,29 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.42578125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
-    <col min="5" max="5" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
     <col min="6" max="6" width="10.85546875" customWidth="1"/>
     <col min="7" max="9" width="7.85546875" customWidth="1"/>
-    <col min="10" max="12" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="10.28515625" customWidth="1"/>
-    <col min="14" max="14" width="11.7109375" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" customWidth="1"/>
-    <col min="16" max="16" width="12.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.42578125" customWidth="1"/>
-    <col min="18" max="18" width="11.28515625" customWidth="1"/>
-    <col min="19" max="19" width="15.140625" customWidth="1"/>
+    <col min="10" max="13" width="11.28515625" customWidth="1"/>
+    <col min="14" max="14" width="4.7109375" customWidth="1"/>
+    <col min="15" max="15" width="11.7109375" customWidth="1"/>
+    <col min="16" max="16" width="11.28515625" customWidth="1"/>
+    <col min="17" max="17" width="12.28515625" customWidth="1"/>
+    <col min="18" max="18" width="13.28515625" customWidth="1"/>
+    <col min="19" max="19" width="11.28515625" customWidth="1"/>
+    <col min="20" max="20" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="P2" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -589,41 +593,44 @@
       <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="1" t="s">
+      <c r="M3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O3" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="O3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="P3" s="1" t="s">
+      <c r="Q3" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O5" s="2" t="s">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P5" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N6" s="1" t="s">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O6" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="O6" s="1" t="s">
+      <c r="P6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="P6" s="1" t="s">
+      <c r="Q6" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E8" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="O8" s="2" t="s">
+      <c r="P8" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -639,38 +646,41 @@
       <c r="E9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="N9" s="1" t="s">
+      <c r="O9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O9" s="1" t="s">
+      <c r="P9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="Q9" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="O11" s="2" t="s">
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="P11" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="N12" s="1" t="s">
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="O12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="O12" s="1" t="s">
+      <c r="P12" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q12" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O14" s="2" t="s">
+      <c r="P14" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>12</v>
       </c>
@@ -686,30 +696,30 @@
       <c r="E15" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="N15" s="1" t="s">
+      <c r="O15" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="O15" s="1" t="s">
+      <c r="P15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="P15" s="1" t="s">
+      <c r="Q15" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="O18" s="2" t="s">
+    <row r="18" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="P18" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="14:16" x14ac:dyDescent="0.25">
-      <c r="N19" s="1" t="s">
+    <row r="19" spans="15:17" x14ac:dyDescent="0.25">
+      <c r="O19" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="O19" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="P19" s="1" t="s">
         <v>36</v>
+      </c>
+      <c r="Q19" s="1" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: convert products from serverside
</commit_message>
<xml_diff>
--- a/docs/sodo_qh.xlsx
+++ b/docs/sodo_qh.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\truon\Desktop\f5mobile-nuxtjs\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2988F2BD-F939-491B-92D4-7AF93F1292EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAF16550-8BAB-4CDA-A2FE-D4CEB5285D94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{11496C9D-87F9-4847-A4DD-6E9F85763FD5}"/>
   </bookViews>
@@ -204,11 +204,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -525,8 +524,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{730279FF-5D8F-42BA-819F-46A5B9217A82}">
   <dimension ref="A2:Q19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="M4" sqref="M4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -593,7 +592,7 @@
       <c r="L3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="1" t="s">
         <v>32</v>
       </c>
       <c r="O3" s="1" t="s">

</xml_diff>